<commit_message>
Extra stuff/components added to the BOM manually
</commit_message>
<xml_diff>
--- a/LKBulls2023_Altium/robonaut-altiumtemplate/BOM/RobonAUT_Project_modified.xlsx
+++ b/LKBulls2023_Altium/robonaut-altiumtemplate/BOM/RobonAUT_Project_modified.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="82">
   <si>
     <t>Item #</t>
   </si>
@@ -228,6 +228,48 @@
   </si>
   <si>
     <t>Quantity</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> + Extra dolgok:</t>
+  </si>
+  <si>
+    <t>43-06-67</t>
+  </si>
+  <si>
+    <t>HÜVELY 20x2 P FHDH2.54-40 (T-T) 1# h=8,5mm AU</t>
+  </si>
+  <si>
+    <t>43-00-12</t>
+  </si>
+  <si>
+    <t>43-00-57</t>
+  </si>
+  <si>
+    <t>43-05-85</t>
+  </si>
+  <si>
+    <t>SZAL.KABEL 6 P ANYA FC-06 (T-T) TEHERMENTESITŐVEL LENGŐ</t>
+  </si>
+  <si>
+    <t>SZAL.KABEL 10 P ANYA FC-10 (T-T) TEHERMENTESITŐVEL LENGŐ</t>
+  </si>
+  <si>
+    <t>SZAL.KABEL 10 P APA 90° BHR-10 (T-T)</t>
+  </si>
+  <si>
+    <t>DS</t>
+  </si>
+  <si>
+    <t>Encoder</t>
+  </si>
+  <si>
+    <t>TÁPCSATL. 2.54mm 4P ANYA HÁZ NCH254-04 (G-S)</t>
+  </si>
+  <si>
+    <t>Bluetooth</t>
+  </si>
+  <si>
+    <t>43-09-08</t>
   </si>
 </sst>
 </file>
@@ -324,7 +366,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -350,6 +392,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normál" xfId="0" builtinId="0"/>
@@ -630,10 +674,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E30"/>
+  <dimension ref="A1:E43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="D44" sqref="D44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1182,7 +1226,118 @@
         <v>3</v>
       </c>
     </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>77</v>
+      </c>
+      <c r="B34" t="s">
+        <v>4</v>
+      </c>
+      <c r="C34" t="s">
+        <v>69</v>
+      </c>
+      <c r="D34" t="s">
+        <v>70</v>
+      </c>
+      <c r="E34">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>77</v>
+      </c>
+      <c r="B35" t="s">
+        <v>4</v>
+      </c>
+      <c r="C35" t="s">
+        <v>71</v>
+      </c>
+      <c r="D35" t="s">
+        <v>74</v>
+      </c>
+      <c r="E35">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>77</v>
+      </c>
+      <c r="B36" t="s">
+        <v>4</v>
+      </c>
+      <c r="C36" t="s">
+        <v>72</v>
+      </c>
+      <c r="D36" t="s">
+        <v>75</v>
+      </c>
+      <c r="E36">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>77</v>
+      </c>
+      <c r="B37" t="s">
+        <v>4</v>
+      </c>
+      <c r="C37" t="s">
+        <v>73</v>
+      </c>
+      <c r="D37" t="s">
+        <v>76</v>
+      </c>
+      <c r="E37">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>78</v>
+      </c>
+      <c r="B38" t="s">
+        <v>4</v>
+      </c>
+      <c r="C38" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="D38" t="s">
+        <v>79</v>
+      </c>
+      <c r="E38">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>80</v>
+      </c>
+      <c r="B39" t="s">
+        <v>4</v>
+      </c>
+      <c r="C39" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="D39" t="s">
+        <v>79</v>
+      </c>
+      <c r="E39">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C43" s="9"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>